<commit_message>
feat: update excel upload to have upsert feature
</commit_message>
<xml_diff>
--- a/app/resources/Employee_List.xlsx
+++ b/app/resources/Employee_List.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darrentan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69C892CA-0DB5-470E-9491-D9B30A734EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4070FCD9-621D-B948-B627-15A723770333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F0368291-BEC8-433A-B4BF-444DCF20852E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F0368291-BEC8-433A-B4BF-444DCF20852E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>END_OF_PROBATION</t>
   </si>
@@ -69,9 +58,6 @@
   </si>
   <si>
     <t>johnny@example.com</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>No</t>
@@ -90,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,21 +464,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -506,7 +492,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -515,7 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -529,16 +515,16 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -552,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>

</xml_diff>